<commit_message>
Tabelas GRASP normalizadas e decodificador
</commit_message>
<xml_diff>
--- a/calibragem/bounded/graspbounded.xlsx
+++ b/calibragem/bounded/graspbounded.xlsx
@@ -538,10 +538,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -549,6 +549,34 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -567,8 +595,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -576,21 +621,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -604,24 +634,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -647,54 +695,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -702,6 +702,84 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -717,67 +795,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -795,37 +819,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -837,7 +861,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -849,37 +873,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -896,6 +896,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -943,8 +967,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -963,168 +996,135 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1133,10 +1133,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -9922,8 +9922,8 @@
   <sheetPr/>
   <dimension ref="A1:D200"/>
   <sheetViews>
-    <sheetView topLeftCell="A171" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12" outlineLevelCol="3"/>
@@ -12740,7 +12740,7 @@
   <dimension ref="A1:D200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:D200"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12" outlineLevelCol="3"/>

</xml_diff>